<commit_message>
excel_merge_neighbors_3.py used group function which works perfectly
</commit_message>
<xml_diff>
--- a/pdtest2.xlsx
+++ b/pdtest2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,33 @@
       <c r="G1" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -480,6 +507,15 @@
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -505,6 +541,15 @@
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -518,14 +563,23 @@
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
+      <c r="D4" t="n">
         <v>4</v>
       </c>
-      <c r="G4" t="n">
+      <c r="E4" t="n">
         <v>0</v>
       </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -551,6 +605,15 @@
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -576,6 +639,15 @@
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -601,6 +673,15 @@
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>